<commit_message>
Added avg, std dev
</commit_message>
<xml_diff>
--- a/Duncan/Atomic-Time/Initial Tests/ArduinoDrift_ard/Analysis of arduino drift.xlsx
+++ b/Duncan/Atomic-Time/Initial Tests/ArduinoDrift_ard/Analysis of arduino drift.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Duncan\Documents\Uni\Documents\Work\2015_16 project\ArduinoDrift_ard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Duncan\Documents\GitHub\Atomic-Time\Duncan\Atomic-Time\Initial Tests\ArduinoDrift_ard\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="print graph" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'print graph'!$A$1:$J$33</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -420,11 +423,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1777122192"/>
-        <c:axId val="1777128720"/>
+        <c:axId val="1113371360"/>
+        <c:axId val="1113372992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1777122192"/>
+        <c:axId val="1113371360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,12 +544,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1777128720"/>
+        <c:crossAx val="1113372992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1777128720"/>
+        <c:axId val="1113372992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.99985999999999997"/>
@@ -665,7 +668,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1777122192"/>
+        <c:crossAx val="1113371360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -926,11 +929,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1777132528"/>
-        <c:axId val="1777120016"/>
+        <c:axId val="1113379520"/>
+        <c:axId val="1113375712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1777132528"/>
+        <c:axId val="1113379520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,12 +1050,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1777120016"/>
+        <c:crossAx val="1113375712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1777120016"/>
+        <c:axId val="1113375712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.99982000000000004"/>
@@ -1172,7 +1175,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1777132528"/>
+        <c:crossAx val="1113379520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1556,13 +1559,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1777124912"/>
-        <c:axId val="1777120560"/>
+        <c:axId val="1113376800"/>
+        <c:axId val="1113377888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1777124912"/>
+        <c:axId val="1113376800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1677,12 +1681,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1777120560"/>
+        <c:crossAx val="1113377888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1777120560"/>
+        <c:axId val="1113377888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.99985999999999997"/>
@@ -1801,7 +1805,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1777124912"/>
+        <c:crossAx val="1113376800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2062,13 +2066,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1378525872"/>
-        <c:axId val="1378519888"/>
+        <c:axId val="1113366464"/>
+        <c:axId val="1367139584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1378525872"/>
+        <c:axId val="1113366464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2183,12 +2188,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1378519888"/>
+        <c:crossAx val="1367139584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1378519888"/>
+        <c:axId val="1367139584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.99982000000000004"/>
@@ -2308,7 +2313,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1378525872"/>
+        <c:crossAx val="1113366464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2352,7 +2357,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -4615,16 +4620,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4658,10 +4663,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>602974</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>165652</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>576470</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>172278</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4686,14 +4691,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>86139</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>26506</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>602974</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>72887</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>569843</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4980,15 +4985,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5002,21 +5010,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
+      <c r="D2">
+        <f>AVERAGE(C:C)</f>
+        <v>0.99980816614795964</v>
+      </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
+      <c r="Q2">
+        <f>AVERAGE(P:P)</f>
+        <v>0.99981229470604116</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>62015</v>
       </c>
@@ -5027,6 +5043,10 @@
         <f>(B3-B2)/(A3-A2)</f>
         <v>0.99983874868983313</v>
       </c>
+      <c r="D3">
+        <f>_xlfn.STDEV.P(C:C)</f>
+        <v>1.2949508210950134E-5</v>
+      </c>
       <c r="N3">
         <v>302010</v>
       </c>
@@ -5037,8 +5057,12 @@
         <f>(O3-O2)/(N3-N2)</f>
         <v>0.99980795337902717</v>
       </c>
+      <c r="Q3">
+        <f>_xlfn.STDEV.P(P:P)</f>
+        <v>2.7633028068528852E-6</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>124026</v>
       </c>
@@ -5060,7 +5084,7 @@
         <v>0.99981126640243967</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>186035</v>
       </c>
@@ -5082,7 +5106,7 @@
         <v>0.99980796037361641</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>248048</v>
       </c>
@@ -5104,7 +5128,7 @@
         <v>0.99981457936003393</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>310067</v>
       </c>
@@ -5126,7 +5150,7 @@
         <v>0.99981126827717737</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>372100</v>
       </c>
@@ -5148,7 +5172,7 @@
         <v>0.99981127452603413</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>434108</v>
       </c>
@@ -5170,7 +5194,7 @@
         <v>0.99980795337902717</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>496123</v>
       </c>
@@ -5192,7 +5216,7 @@
         <v>0.99981457936003393</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>558136</v>
       </c>
@@ -5214,7 +5238,7 @@
         <v>0.99981126077800297</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>620149</v>
       </c>
@@ -5236,7 +5260,7 @@
         <v>0.99981127452603413</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>682154</v>
       </c>
@@ -5258,7 +5282,7 @@
         <v>0.99981457813213959</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>744167</v>
       </c>
@@ -5280,7 +5304,7 @@
         <v>0.99981126515259378</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>806182</v>
       </c>
@@ -5302,7 +5326,7 @@
         <v>0.99981126827717737</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>868201</v>
       </c>
@@ -5664,14 +5688,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>